<commit_message>
update gitignore and data tracking
</commit_message>
<xml_diff>
--- a/data mamagement.xlsx
+++ b/data mamagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy/projects/Teebloc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31822033-A360-9B4E-9E28-FF6B34D79B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1813B2F5-033E-A446-98A1-D57FF556D9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="3960" windowWidth="24460" windowHeight="16180" xr2:uid="{5E373B72-7875-214D-9DE2-95D517138179}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="452">
   <si>
     <t>https://www.testpapersfree.com/pdfs/P4_Maths_2022_SA1_acsprimary.pdf</t>
   </si>
@@ -1151,9 +1151,6 @@
     <t>https://www.testpapersfree.com/pdfs/P5_Science_2023_WA2_nanhua.pdf</t>
   </si>
   <si>
-    <t>https://www.testpapersfree.com/pdfs/P5_Science_2023_SA2_Raffles.pdf HEREE</t>
-  </si>
-  <si>
     <t>https://www.testpapersfree.com/pdfs/P5_Science_2023_SA2_Nanyang.pdf</t>
   </si>
   <si>
@@ -1370,9 +1367,6 @@
     <t>https://www.testpapersfree.com/pdfs/P6_Maths_2023_SA2_Temasek.pdf</t>
   </si>
   <si>
-    <t>https://www.testpapersfree.com/pdfs/P6_Maths_2023_SA2_Taonan.pdf HERE</t>
-  </si>
-  <si>
     <t>paper</t>
   </si>
   <si>
@@ -1389,16 +1383,33 @@
   </si>
   <si>
     <t>OE new</t>
+  </si>
+  <si>
+    <t>cascading</t>
+  </si>
+  <si>
+    <t>https://www.testpapersfree.com/pdfs/P5_Science_2023_SA2_Raffles.pdf</t>
+  </si>
+  <si>
+    <t>https://www.testpapersfree.com/pdfs/P6_Maths_2023_SA2_Taonan.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1427,14 +1438,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1767,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FDCE66-0A14-4A4D-A206-6CE028C84DF5}">
-  <dimension ref="A1:F447"/>
+  <dimension ref="A1:G447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="B337" sqref="B337"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="G418" sqref="G418:G447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,97 +1794,100 @@
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C1" t="s">
         <v>445</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>446</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>447</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>448</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>449</v>
       </c>
-      <c r="F1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3075,860 +3092,986 @@
         <v>253</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G260" s="1"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G261" s="1"/>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G262" s="1"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G263" s="1"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G264" s="1"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G265" s="1"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G266" s="1"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G267" s="1"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G268" s="1"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G269" s="1"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G270" s="1"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G271" s="1"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G272" s="1"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G273" s="1"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G274" s="1"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G275" s="1"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G276" s="1"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G277" s="1"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G278" s="1"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G279" s="1"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G280" s="1"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G281" s="1"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G282" s="1"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G283" s="1"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G284" s="1"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G285" s="1"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G286" s="1"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G287" s="1"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G288" s="1"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G289" s="1"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G290" s="1"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G291" s="1"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G292" s="1"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G293" s="1"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G294" s="1"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G295" s="1"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G296" s="1"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G297" s="1"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G298" s="1"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G299" s="1"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G300" s="1"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G301" s="1"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G302" s="1"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G303" s="1"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G304" s="1"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G305" s="1"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G306" s="1"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G307" s="1"/>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G308" s="1"/>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G309" s="1"/>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G310" s="1"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G311" s="1"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G312" s="1"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G313" s="1"/>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G314" s="1"/>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G315" s="1"/>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G316" s="1"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G317" s="1"/>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G318" s="1"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G319" s="1"/>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G320" s="1"/>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G321" s="1"/>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G322" s="1"/>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G323" s="1"/>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G324" s="1"/>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G325" s="1"/>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G326" s="1"/>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G327" s="1"/>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G328" s="1"/>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G329" s="1"/>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G330" s="1"/>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G331" s="1"/>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G332" s="1"/>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G333" s="1"/>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G334" s="1"/>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G335" s="1"/>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G336" s="1"/>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G337" s="1"/>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G338" s="1"/>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G339" s="1"/>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G340" s="1"/>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G341" s="1"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G342" s="1"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G343" s="1"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G344" s="1"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G345" s="1"/>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G346" s="1"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G347" s="1"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G348" s="1"/>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G349" s="1"/>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G350" s="1"/>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G351" s="1"/>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G352" s="1"/>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G353" s="1"/>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>351</v>
       </c>
       <c r="F354" s="1"/>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G354" s="1"/>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>352</v>
       </c>
       <c r="F355" s="1"/>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G355" s="1"/>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>353</v>
       </c>
       <c r="F356" s="1"/>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G356" s="1"/>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>354</v>
       </c>
       <c r="F357" s="1"/>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G357" s="1"/>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>355</v>
       </c>
       <c r="F358" s="1"/>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G358" s="1"/>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>356</v>
       </c>
       <c r="F359" s="1"/>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G359" s="1"/>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>357</v>
       </c>
       <c r="F360" s="1"/>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G360" s="1"/>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>358</v>
       </c>
       <c r="F361" s="1"/>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G361" s="1"/>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>359</v>
       </c>
       <c r="F362" s="1"/>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G362" s="1"/>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>360</v>
       </c>
       <c r="F363" s="1"/>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G363" s="1"/>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>361</v>
       </c>
       <c r="F364" s="1"/>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G364" s="1"/>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>362</v>
       </c>
       <c r="F365" s="1"/>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G365" s="1"/>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>363</v>
       </c>
       <c r="F366" s="1"/>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G366" s="1"/>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>364</v>
       </c>
       <c r="F367" s="1"/>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G367" s="1"/>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>365</v>
       </c>
       <c r="F368" s="1"/>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G368" s="1"/>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>366</v>
       </c>
       <c r="F369" s="1"/>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G369" s="1"/>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>367</v>
       </c>
       <c r="F370" s="1"/>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G370" s="1"/>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>368</v>
       </c>
       <c r="F371" s="1"/>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G371" s="1"/>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>369</v>
       </c>
       <c r="F372" s="1"/>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G372" s="1"/>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>370</v>
       </c>
       <c r="F373" s="1"/>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A374" t="s">
-        <v>371</v>
+      <c r="G373" s="1"/>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A374" s="2" t="s">
+        <v>450</v>
       </c>
       <c r="B374" s="1"/>
       <c r="C374" s="1"/>
       <c r="D374" s="1"/>
       <c r="E374" s="1"/>
       <c r="F374" s="1"/>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G374" s="1"/>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B375" s="1"/>
       <c r="C375" s="1"/>
       <c r="D375" s="1"/>
       <c r="E375" s="1"/>
       <c r="F375" s="1"/>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G375" s="1"/>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B376" s="1"/>
       <c r="C376" s="1"/>
       <c r="D376" s="1"/>
       <c r="E376" s="1"/>
       <c r="F376" s="1"/>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G376" s="1"/>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B377" s="1"/>
       <c r="C377" s="1"/>
       <c r="D377" s="1"/>
       <c r="E377" s="1"/>
       <c r="F377" s="1"/>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G377" s="1"/>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B378" s="1"/>
       <c r="C378" s="1"/>
       <c r="D378" s="1"/>
       <c r="E378" s="1"/>
       <c r="F378" s="1"/>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G378" s="1"/>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B379" s="1"/>
       <c r="C379" s="1"/>
       <c r="D379" s="1"/>
       <c r="E379" s="1"/>
       <c r="F379" s="1"/>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G379" s="1"/>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B380" s="1"/>
       <c r="C380" s="1"/>
       <c r="D380" s="1"/>
       <c r="E380" s="1"/>
       <c r="F380" s="1"/>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G380" s="1"/>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B381" s="1"/>
       <c r="C381" s="1"/>
       <c r="D381" s="1"/>
       <c r="E381" s="1"/>
       <c r="F381" s="1"/>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G381" s="1"/>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B382" s="1"/>
       <c r="C382" s="1"/>
       <c r="D382" s="1"/>
       <c r="E382" s="1"/>
       <c r="F382" s="1"/>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G382" s="1"/>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B383" s="1"/>
       <c r="C383" s="1"/>
       <c r="D383" s="1"/>
       <c r="E383" s="1"/>
       <c r="F383" s="1"/>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G383" s="1"/>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B384" s="1"/>
       <c r="C384" s="1"/>
       <c r="D384" s="1"/>
       <c r="E384" s="1"/>
       <c r="F384" s="1"/>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G384" s="1"/>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B385" s="1"/>
       <c r="C385" s="1"/>
       <c r="D385" s="1"/>
       <c r="E385" s="1"/>
       <c r="F385" s="1"/>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G385" s="1"/>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B386" s="1"/>
       <c r="D386" s="1"/>
       <c r="E386" s="1"/>
       <c r="F386" s="1"/>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B387" s="1"/>
       <c r="D387" s="1"/>
       <c r="E387" s="1"/>
       <c r="F387" s="1"/>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B388" s="1"/>
       <c r="D388" s="1"/>
       <c r="E388" s="1"/>
       <c r="F388" s="1"/>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B389" s="1"/>
       <c r="D389" s="1"/>
       <c r="E389" s="1"/>
       <c r="F389" s="1"/>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B390" s="1"/>
       <c r="D390" s="1"/>
       <c r="E390" s="1"/>
       <c r="F390" s="1"/>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B391" s="1"/>
       <c r="D391" s="1"/>
       <c r="E391" s="1"/>
       <c r="F391" s="1"/>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B392" s="1"/>
       <c r="D392" s="1"/>
       <c r="E392" s="1"/>
       <c r="F392" s="1"/>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B393" s="1"/>
       <c r="D393" s="1"/>
       <c r="E393" s="1"/>
       <c r="F393" s="1"/>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B394" s="1"/>
       <c r="D394" s="1"/>
       <c r="E394" s="1"/>
       <c r="F394" s="1"/>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B395" s="1"/>
       <c r="D395" s="1"/>
       <c r="E395" s="1"/>
       <c r="F395" s="1"/>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B396" s="1"/>
       <c r="D396" s="1"/>
       <c r="E396" s="1"/>
       <c r="F396" s="1"/>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B397" s="1"/>
       <c r="D397" s="1"/>
       <c r="E397" s="1"/>
       <c r="F397" s="1"/>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B398" s="1"/>
       <c r="D398" s="1"/>
       <c r="E398" s="1"/>
       <c r="F398" s="1"/>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B399" s="1"/>
       <c r="D399" s="1"/>
       <c r="E399" s="1"/>
       <c r="F399" s="1"/>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B400" s="1"/>
       <c r="D400" s="1"/>
@@ -3937,7 +4080,7 @@
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B401" s="1"/>
       <c r="D401" s="1"/>
@@ -3946,7 +4089,7 @@
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B402" s="1"/>
       <c r="D402" s="1"/>
@@ -3955,7 +4098,7 @@
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B403" s="1"/>
       <c r="D403" s="1"/>
@@ -3964,7 +4107,7 @@
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B404" s="1"/>
       <c r="D404" s="1"/>
@@ -3973,7 +4116,7 @@
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B405" s="1"/>
       <c r="D405" s="1"/>
@@ -3982,7 +4125,7 @@
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B406" s="1"/>
       <c r="D406" s="1"/>
@@ -3991,7 +4134,7 @@
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B407" s="1"/>
       <c r="D407" s="1"/>
@@ -4000,7 +4143,7 @@
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B408" s="1"/>
       <c r="D408" s="1"/>
@@ -4009,7 +4152,7 @@
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B409" s="1"/>
       <c r="D409" s="1"/>
@@ -4018,7 +4161,7 @@
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B410" s="1"/>
       <c r="D410" s="1"/>
@@ -4027,7 +4170,7 @@
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B411" s="1"/>
       <c r="D411" s="1"/>
@@ -4036,7 +4179,7 @@
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B412" s="1"/>
       <c r="D412" s="1"/>
@@ -4045,7 +4188,7 @@
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B413" s="1"/>
       <c r="D413" s="1"/>
@@ -4054,7 +4197,7 @@
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B414" s="1"/>
       <c r="D414" s="1"/>
@@ -4063,7 +4206,7 @@
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B415" s="1"/>
       <c r="D415" s="1"/>
@@ -4072,293 +4215,327 @@
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B416" s="1"/>
       <c r="D416" s="1"/>
       <c r="E416" s="1"/>
       <c r="F416" s="1"/>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B417" s="1"/>
       <c r="D417" s="1"/>
       <c r="E417" s="1"/>
       <c r="F417" s="1"/>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B418" s="1"/>
       <c r="D418" s="1"/>
       <c r="E418" s="1"/>
       <c r="F418" s="1"/>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G418" s="1"/>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B419" s="1"/>
       <c r="D419" s="1"/>
       <c r="E419" s="1"/>
       <c r="F419" s="1"/>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G419" s="1"/>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B420" s="1"/>
       <c r="D420" s="1"/>
       <c r="E420" s="1"/>
       <c r="F420" s="1"/>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G420" s="1"/>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B421" s="1"/>
       <c r="D421" s="1"/>
       <c r="E421" s="1"/>
       <c r="F421" s="1"/>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G421" s="1"/>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B422" s="1"/>
       <c r="D422" s="1"/>
       <c r="E422" s="1"/>
       <c r="F422" s="1"/>
-    </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G422" s="1"/>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B423" s="1"/>
       <c r="D423" s="1"/>
       <c r="E423" s="1"/>
       <c r="F423" s="1"/>
-    </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G423" s="1"/>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B424" s="1"/>
       <c r="D424" s="1"/>
       <c r="E424" s="1"/>
       <c r="F424" s="1"/>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G424" s="1"/>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B425" s="1"/>
       <c r="D425" s="1"/>
       <c r="E425" s="1"/>
       <c r="F425" s="1"/>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G425" s="1"/>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B426" s="1"/>
       <c r="D426" s="1"/>
       <c r="E426" s="1"/>
       <c r="F426" s="1"/>
-    </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G426" s="1"/>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B427" s="1"/>
       <c r="D427" s="1"/>
       <c r="E427" s="1"/>
       <c r="F427" s="1"/>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G427" s="1"/>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B428" s="1"/>
       <c r="D428" s="1"/>
       <c r="E428" s="1"/>
       <c r="F428" s="1"/>
-    </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G428" s="1"/>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B429" s="1"/>
       <c r="D429" s="1"/>
       <c r="E429" s="1"/>
       <c r="F429" s="1"/>
-    </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G429" s="1"/>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B430" s="1"/>
       <c r="D430" s="1"/>
       <c r="E430" s="1"/>
       <c r="F430" s="1"/>
-    </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G430" s="1"/>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B431" s="1"/>
       <c r="C431" s="1"/>
       <c r="D431" s="1"/>
       <c r="F431" s="1"/>
-    </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G431" s="1"/>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B432" s="1"/>
       <c r="C432" s="1"/>
       <c r="D432" s="1"/>
       <c r="F432" s="1"/>
-    </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G432" s="1"/>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B433" s="1"/>
       <c r="C433" s="1"/>
       <c r="D433" s="1"/>
       <c r="F433" s="1"/>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G433" s="1"/>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B434" s="1"/>
       <c r="C434" s="1"/>
       <c r="D434" s="1"/>
       <c r="F434" s="1"/>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G434" s="1"/>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B435" s="1"/>
       <c r="C435" s="1"/>
       <c r="D435" s="1"/>
       <c r="F435" s="1"/>
-    </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G435" s="1"/>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B436" s="1"/>
       <c r="C436" s="1"/>
       <c r="D436" s="1"/>
       <c r="F436" s="1"/>
-    </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G436" s="1"/>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B437" s="1"/>
       <c r="C437" s="1"/>
       <c r="D437" s="1"/>
       <c r="F437" s="1"/>
-    </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G437" s="1"/>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B438" s="1"/>
       <c r="C438" s="1"/>
       <c r="D438" s="1"/>
       <c r="F438" s="1"/>
-    </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G438" s="1"/>
+    </row>
+    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B439" s="1"/>
       <c r="C439" s="1"/>
       <c r="D439" s="1"/>
       <c r="F439" s="1"/>
-    </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G439" s="1"/>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B440" s="1"/>
       <c r="C440" s="1"/>
       <c r="D440" s="1"/>
       <c r="F440" s="1"/>
-    </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G440" s="1"/>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B441" s="1"/>
       <c r="C441" s="1"/>
       <c r="D441" s="1"/>
       <c r="F441" s="1"/>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G441" s="1"/>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B442" s="1"/>
       <c r="C442" s="1"/>
       <c r="D442" s="1"/>
       <c r="F442" s="1"/>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G442" s="1"/>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B443" s="1"/>
       <c r="C443" s="1"/>
       <c r="D443" s="1"/>
       <c r="F443" s="1"/>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G443" s="1"/>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B444" s="1"/>
       <c r="C444" s="1"/>
       <c r="D444" s="1"/>
       <c r="F444" s="1"/>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G444" s="1"/>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B445" s="1"/>
       <c r="C445" s="1"/>
       <c r="D445" s="1"/>
       <c r="F445" s="1"/>
-    </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G445" s="1"/>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B446" s="1"/>
       <c r="C446" s="1"/>
       <c r="D446" s="1"/>
       <c r="F446" s="1"/>
-    </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A447" t="s">
-        <v>444</v>
+      <c r="G446" s="1"/>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A447" s="2" t="s">
+        <v>451</v>
       </c>
       <c r="B447" s="1"/>
       <c r="C447" s="1"/>
       <c r="D447" s="1"/>
       <c r="F447" s="1"/>
+      <c r="G447" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A374" r:id="rId1" xr:uid="{F691C518-683A-5741-8747-31D3531EFC97}"/>
+    <hyperlink ref="A447" r:id="rId2" xr:uid="{D7D5E5B3-AB45-DB45-B479-AC0E02BEC9B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
modified cascade Classifier's psuedolabelling script to train on confidence <0.6
</commit_message>
<xml_diff>
--- a/data mamagement.xlsx
+++ b/data mamagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy/projects/Teebloc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1813B2F5-033E-A446-98A1-D57FF556D9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98D95BD-F609-1545-B75E-A9C51E1BFD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="3960" windowWidth="24460" windowHeight="16180" xr2:uid="{5E373B72-7875-214D-9DE2-95D517138179}"/>
   </bookViews>
@@ -1783,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FDCE66-0A14-4A4D-A206-6CE028C84DF5}">
   <dimension ref="A1:G447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
-      <selection activeCell="G418" sqref="G418:G447"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1821,1291 +1821,1549 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G101" s="1"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G102" s="1"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G103" s="1"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G104" s="1"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G105" s="1"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G106" s="1"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G107" s="1"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G108" s="1"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G110" s="1"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G111" s="1"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G112" s="1"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G113" s="1"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G114" s="1"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G115" s="1"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G116" s="1"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G117" s="1"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G118" s="1"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G119" s="1"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G120" s="1"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G121" s="1"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G122" s="1"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G123" s="1"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G124" s="1"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G125" s="1"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G126" s="1"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G127" s="1"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G128" s="1"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G129" s="1"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G130" s="1"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G131" s="1"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G132" s="1"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G133" s="1"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G134" s="1"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G135" s="1"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G136" s="1"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G137" s="1"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G138" s="1"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G139" s="1"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G140" s="1"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G141" s="1"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G142" s="1"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G143" s="1"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G144" s="1"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G145" s="1"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G146" s="1"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G147" s="1"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G148" s="1"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G149" s="1"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G150" s="1"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G151" s="1"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G152" s="1"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G153" s="1"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G154" s="1"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G155" s="1"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G156" s="1"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G157" s="1"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G158" s="1"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G159" s="1"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G160" s="1"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G161" s="1"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G162" s="1"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G163" s="1"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G164" s="1"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G165" s="1"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G166" s="1"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G167" s="1"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G168" s="1"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G169" s="1"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G170" s="1"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G171" s="1"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G172" s="1"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G173" s="1"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G174" s="1"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G175" s="1"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G176" s="1"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G177" s="1"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G178" s="1"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G179" s="1"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G180" s="1"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G181" s="1"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G182" s="1"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G183" s="1"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G184" s="1"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G185" s="1"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G186" s="1"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G187" s="1"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G188" s="1"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G189" s="1"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G190" s="1"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G191" s="1"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G192" s="1"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G193" s="1"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G194" s="1"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G195" s="1"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G196" s="1"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G197" s="1"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G198" s="1"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G199" s="1"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G200" s="1"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G201" s="1"/>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G202" s="1"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G203" s="1"/>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G204" s="1"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G205" s="1"/>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G206" s="1"/>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G207" s="1"/>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G208" s="1"/>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G209" s="1"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G210" s="1"/>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G211" s="1"/>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G212" s="1"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G213" s="1"/>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G214" s="1"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G215" s="1"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G216" s="1"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G217" s="1"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G218" s="1"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G219" s="1"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G220" s="1"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G221" s="1"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G222" s="1"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G223" s="1"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G224" s="1"/>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G225" s="1"/>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G226" s="1"/>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G227" s="1"/>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G228" s="1"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G229" s="1"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G230" s="1"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G231" s="1"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G232" s="1"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G233" s="1"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G234" s="1"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G235" s="1"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G236" s="1"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G237" s="1"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G238" s="1"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G239" s="1"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G240" s="1"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G241" s="1"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G242" s="1"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G243" s="1"/>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G244" s="1"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G245" s="1"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G246" s="1"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G247" s="1"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G248" s="1"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G249" s="1"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G250" s="1"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G251" s="1"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G252" s="1"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G253" s="1"/>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G254" s="1"/>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G255" s="1"/>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>253</v>
       </c>
+      <c r="G256" s="1"/>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>254</v>
       </c>
+      <c r="G257" s="1"/>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>255</v>
       </c>
+      <c r="G258" s="1"/>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>256</v>
       </c>
+      <c r="G259" s="1"/>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
@@ -3951,6 +4209,7 @@
       <c r="D386" s="1"/>
       <c r="E386" s="1"/>
       <c r="F386" s="1"/>
+      <c r="G386" s="1"/>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
@@ -3960,6 +4219,7 @@
       <c r="D387" s="1"/>
       <c r="E387" s="1"/>
       <c r="F387" s="1"/>
+      <c r="G387" s="1"/>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
@@ -3969,6 +4229,7 @@
       <c r="D388" s="1"/>
       <c r="E388" s="1"/>
       <c r="F388" s="1"/>
+      <c r="G388" s="1"/>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
@@ -3978,6 +4239,7 @@
       <c r="D389" s="1"/>
       <c r="E389" s="1"/>
       <c r="F389" s="1"/>
+      <c r="G389" s="1"/>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
@@ -3987,6 +4249,7 @@
       <c r="D390" s="1"/>
       <c r="E390" s="1"/>
       <c r="F390" s="1"/>
+      <c r="G390" s="1"/>
     </row>
     <row r="391" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
@@ -3996,6 +4259,7 @@
       <c r="D391" s="1"/>
       <c r="E391" s="1"/>
       <c r="F391" s="1"/>
+      <c r="G391" s="1"/>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
@@ -4005,6 +4269,7 @@
       <c r="D392" s="1"/>
       <c r="E392" s="1"/>
       <c r="F392" s="1"/>
+      <c r="G392" s="1"/>
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
@@ -4014,6 +4279,7 @@
       <c r="D393" s="1"/>
       <c r="E393" s="1"/>
       <c r="F393" s="1"/>
+      <c r="G393" s="1"/>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
@@ -4023,6 +4289,7 @@
       <c r="D394" s="1"/>
       <c r="E394" s="1"/>
       <c r="F394" s="1"/>
+      <c r="G394" s="1"/>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
@@ -4032,6 +4299,7 @@
       <c r="D395" s="1"/>
       <c r="E395" s="1"/>
       <c r="F395" s="1"/>
+      <c r="G395" s="1"/>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
@@ -4041,6 +4309,7 @@
       <c r="D396" s="1"/>
       <c r="E396" s="1"/>
       <c r="F396" s="1"/>
+      <c r="G396" s="1"/>
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
@@ -4050,6 +4319,7 @@
       <c r="D397" s="1"/>
       <c r="E397" s="1"/>
       <c r="F397" s="1"/>
+      <c r="G397" s="1"/>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
@@ -4059,6 +4329,7 @@
       <c r="D398" s="1"/>
       <c r="E398" s="1"/>
       <c r="F398" s="1"/>
+      <c r="G398" s="1"/>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
@@ -4068,6 +4339,7 @@
       <c r="D399" s="1"/>
       <c r="E399" s="1"/>
       <c r="F399" s="1"/>
+      <c r="G399" s="1"/>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
@@ -4077,8 +4349,9 @@
       <c r="D400" s="1"/>
       <c r="E400" s="1"/>
       <c r="F400" s="1"/>
-    </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G400" s="1"/>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>397</v>
       </c>
@@ -4086,8 +4359,9 @@
       <c r="D401" s="1"/>
       <c r="E401" s="1"/>
       <c r="F401" s="1"/>
-    </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G401" s="1"/>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>398</v>
       </c>
@@ -4095,8 +4369,9 @@
       <c r="D402" s="1"/>
       <c r="E402" s="1"/>
       <c r="F402" s="1"/>
-    </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G402" s="1"/>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>399</v>
       </c>
@@ -4104,8 +4379,9 @@
       <c r="D403" s="1"/>
       <c r="E403" s="1"/>
       <c r="F403" s="1"/>
-    </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G403" s="1"/>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>400</v>
       </c>
@@ -4113,8 +4389,9 @@
       <c r="D404" s="1"/>
       <c r="E404" s="1"/>
       <c r="F404" s="1"/>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G404" s="1"/>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>401</v>
       </c>
@@ -4122,8 +4399,9 @@
       <c r="D405" s="1"/>
       <c r="E405" s="1"/>
       <c r="F405" s="1"/>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G405" s="1"/>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>402</v>
       </c>
@@ -4131,8 +4409,9 @@
       <c r="D406" s="1"/>
       <c r="E406" s="1"/>
       <c r="F406" s="1"/>
-    </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G406" s="1"/>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>403</v>
       </c>
@@ -4140,8 +4419,9 @@
       <c r="D407" s="1"/>
       <c r="E407" s="1"/>
       <c r="F407" s="1"/>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G407" s="1"/>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>404</v>
       </c>
@@ -4149,8 +4429,9 @@
       <c r="D408" s="1"/>
       <c r="E408" s="1"/>
       <c r="F408" s="1"/>
-    </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G408" s="1"/>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>405</v>
       </c>
@@ -4158,8 +4439,9 @@
       <c r="D409" s="1"/>
       <c r="E409" s="1"/>
       <c r="F409" s="1"/>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G409" s="1"/>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>406</v>
       </c>
@@ -4167,8 +4449,9 @@
       <c r="D410" s="1"/>
       <c r="E410" s="1"/>
       <c r="F410" s="1"/>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G410" s="1"/>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>407</v>
       </c>
@@ -4176,8 +4459,9 @@
       <c r="D411" s="1"/>
       <c r="E411" s="1"/>
       <c r="F411" s="1"/>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G411" s="1"/>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>408</v>
       </c>
@@ -4185,8 +4469,9 @@
       <c r="D412" s="1"/>
       <c r="E412" s="1"/>
       <c r="F412" s="1"/>
-    </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G412" s="1"/>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>409</v>
       </c>
@@ -4194,8 +4479,9 @@
       <c r="D413" s="1"/>
       <c r="E413" s="1"/>
       <c r="F413" s="1"/>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G413" s="1"/>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>410</v>
       </c>
@@ -4203,8 +4489,9 @@
       <c r="D414" s="1"/>
       <c r="E414" s="1"/>
       <c r="F414" s="1"/>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G414" s="1"/>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>411</v>
       </c>
@@ -4212,8 +4499,9 @@
       <c r="D415" s="1"/>
       <c r="E415" s="1"/>
       <c r="F415" s="1"/>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G415" s="1"/>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>412</v>
       </c>
@@ -4221,6 +4509,7 @@
       <c r="D416" s="1"/>
       <c r="E416" s="1"/>
       <c r="F416" s="1"/>
+      <c r="G416" s="1"/>
     </row>
     <row r="417" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
@@ -4230,6 +4519,7 @@
       <c r="D417" s="1"/>
       <c r="E417" s="1"/>
       <c r="F417" s="1"/>
+      <c r="G417" s="1"/>
     </row>
     <row r="418" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A418" t="s">

</xml_diff>